<commit_message>
Update Product Backlog Sprint 2.xlsx
</commit_message>
<xml_diff>
--- a/Documentos/Product Backlog Sprint 2.xlsx
+++ b/Documentos/Product Backlog Sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtorr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D11C6DA6-1B28-4E3A-9A8C-4B4EFB8BA428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ED2E904-8049-4770-A30D-B8F501AE962E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId14"/>
+    <pivotCache cacheId="4" r:id="rId14"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -259,9 +259,6 @@
     <t>Diego Natividad</t>
   </si>
   <si>
-    <t>pendiente</t>
-  </si>
-  <si>
     <t>Crear formulario de Login</t>
   </si>
   <si>
@@ -468,16 +465,26 @@
   <si>
     <t>Estimación por Lógica Difusa</t>
   </si>
+  <si>
+    <t>completado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -732,126 +739,127 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7448,7 +7456,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B23:C29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -7761,16 +7769,16 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:25" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -7778,34 +7786,34 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44" t="s">
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="55" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="22" t="s">
         <v>9</v>
       </c>
@@ -7815,9 +7823,9 @@
       <c r="F7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -7836,7 +7844,7 @@
       <c r="Y7" s="6"/>
     </row>
     <row r="8" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="47" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="24" t="s">
@@ -7865,7 +7873,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="24" t="s">
         <v>18</v>
       </c>
@@ -7892,7 +7900,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="49" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -7921,7 +7929,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="24" t="s">
         <v>29</v>
       </c>
@@ -7948,7 +7956,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="24" t="s">
         <v>31</v>
       </c>
@@ -7976,7 +7984,7 @@
     </row>
     <row r="13" spans="1:25" ht="57" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>35</v>
@@ -8004,14 +8012,14 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
-        <v>90</v>
+      <c r="A14" s="38" t="s">
+        <v>89</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>26</v>
@@ -8033,7 +8041,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="24" t="s">
         <v>43</v>
       </c>
@@ -8060,8 +8068,8 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="49" t="s">
-        <v>94</v>
+      <c r="A16" s="38" t="s">
+        <v>93</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>46</v>
@@ -8089,12 +8097,12 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="24" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>20</v>
@@ -8116,23 +8124,23 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
-        <v>105</v>
+      <c r="A18" s="37" t="s">
+        <v>104</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="29">
         <v>40</v>
@@ -8145,26 +8153,26 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="48"/>
-      <c r="B19" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="32" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="45">
+      <c r="E19" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="41">
         <v>40</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="41">
         <v>3</v>
       </c>
       <c r="I19" s="27" t="s">
@@ -8172,39 +8180,39 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="23" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
       <c r="I20" s="27" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="10" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
-      <c r="B21" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="51" t="s">
+      <c r="A21" s="37"/>
+      <c r="B21" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="51" t="s">
+      <c r="F21" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="47">
+      <c r="G21" s="36">
         <v>20</v>
       </c>
-      <c r="H21" s="47">
+      <c r="H21" s="36">
         <v>3</v>
       </c>
       <c r="I21" s="27" t="s">
@@ -8212,14 +8220,14 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="10" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="27" t="s">
         <v>31</v>
       </c>
@@ -13036,6 +13044,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="A18:A22"/>
@@ -13052,19 +13071,8 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="G19:G20"/>
   </mergeCells>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I8" location="'HU001'!A1" display="HU001" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="I9" location="'HU002'!A1" display="HU002" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -13214,7 +13222,7 @@
   <dimension ref="B2:J41"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="F3" sqref="F3:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13269,13 +13277,13 @@
         <v>67</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>70</v>
+      <c r="F3" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G3" s="13">
         <f>(H3+I3+4*J3)/6</f>
@@ -13304,8 +13312,8 @@
       <c r="E4" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>70</v>
+      <c r="F4" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G4" s="13">
         <f>(H4+I4+4*J4)/6</f>
@@ -13329,13 +13337,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>70</v>
+      <c r="F5" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G5" s="13">
         <f>(H5+I5+4*J5)/6</f>
@@ -13359,13 +13367,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G21" si="0">(H6+I6+4*J6)/6</f>
@@ -13389,13 +13397,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
@@ -13419,13 +13427,13 @@
         <v>19</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
@@ -13449,13 +13457,13 @@
         <v>25</v>
       </c>
       <c r="D9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>70</v>
+      <c r="F9" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
@@ -13479,13 +13487,13 @@
         <v>25</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
@@ -13509,13 +13517,13 @@
         <v>25</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
@@ -13539,13 +13547,13 @@
         <v>30</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>70</v>
+      <c r="F12" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G12" s="13">
         <f t="shared" si="0"/>
@@ -13569,13 +13577,13 @@
         <v>30</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G13" s="13">
         <f t="shared" si="0"/>
@@ -13599,13 +13607,13 @@
         <v>30</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G14" s="13">
         <f t="shared" si="0"/>
@@ -13629,13 +13637,13 @@
         <v>32</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" si="0"/>
@@ -13659,13 +13667,13 @@
         <v>32</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G16" s="13">
         <f t="shared" si="0"/>
@@ -13689,13 +13697,13 @@
         <v>36</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G17" s="13">
         <f t="shared" si="0"/>
@@ -13719,13 +13727,13 @@
         <v>36</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G18" s="13">
         <f t="shared" si="0"/>
@@ -13749,13 +13757,13 @@
         <v>40</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G19" s="13">
         <f t="shared" si="0"/>
@@ -13779,13 +13787,13 @@
         <v>40</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G20" s="13">
         <f t="shared" si="0"/>
@@ -13809,13 +13817,13 @@
         <v>40</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="G21" s="13">
         <f t="shared" si="0"/>
@@ -13837,17 +13845,17 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="15"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="21">
         <v>9.8333333333333339</v>
@@ -13865,7 +13873,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="21">
         <v>8.4166666666666661</v>
@@ -13874,7 +13882,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="21">
         <v>8.75</v>
@@ -13883,7 +13891,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="21">
         <v>10.583333333333332</v>
@@ -13892,7 +13900,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="21">
         <v>46.325000000000003</v>
@@ -13969,7 +13977,7 @@
   <dimension ref="C2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G3" sqref="G3:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13987,23 +13995,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="54" t="s">
-        <v>139</v>
+      <c r="H2" s="34" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
@@ -14011,126 +14019,126 @@
         <v>39</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="55">
+        <v>74</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="35">
         <v>0.27</v>
       </c>
-      <c r="I3" s="52"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>108</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>109</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>70</v>
+      <c r="G4" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H4" s="12">
         <v>0.35</v>
       </c>
-      <c r="I4" s="52"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H5" s="12">
         <v>0.27</v>
       </c>
-      <c r="I5" s="52"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H6" s="12">
         <v>0.22</v>
       </c>
-      <c r="I6" s="52"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="31" t="s">
-        <v>70</v>
+      <c r="G7" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H7" s="12">
         <v>0.32</v>
       </c>
-      <c r="I7" s="52"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H8" s="12">
         <v>0.35</v>
       </c>
-      <c r="I8" s="52"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
@@ -14140,18 +14148,18 @@
         <v>47</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H9" s="12">
         <v>0.24</v>
       </c>
-      <c r="I9" s="52"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="31" t="s">
@@ -14161,18 +14169,18 @@
         <v>47</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>70</v>
+      <c r="G10" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H10" s="12">
         <v>0.38</v>
       </c>
-      <c r="I10" s="52"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="31" t="s">
@@ -14182,18 +14190,18 @@
         <v>47</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H11" s="12">
         <v>0.32</v>
       </c>
-      <c r="I11" s="52"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="31" t="s">
@@ -14203,18 +14211,18 @@
         <v>47</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H12" s="12">
         <v>0.27</v>
       </c>
-      <c r="I12" s="52"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="31" t="s">
@@ -14224,18 +14232,18 @@
         <v>47</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>70</v>
+      <c r="G13" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H13" s="12">
         <v>0.38</v>
       </c>
-      <c r="I13" s="52"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
@@ -14245,19 +14253,19 @@
         <v>47</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H14" s="12">
         <v>0.25</v>
       </c>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="31" t="s">
@@ -14267,19 +14275,19 @@
         <v>51</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H15" s="12">
         <v>0.23</v>
       </c>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="31" t="s">
@@ -14289,18 +14297,18 @@
         <v>51</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="31" t="s">
-        <v>70</v>
+      <c r="G16" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H16" s="12">
         <v>0.41</v>
       </c>
-      <c r="I16" s="52"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="31" t="s">
@@ -14310,34 +14318,34 @@
         <v>51</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H17" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J17" s="52"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="31" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H18" s="12">
         <v>0.18</v>
@@ -14348,42 +14356,42 @@
         <v>50</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>70</v>
+      <c r="G19" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H19" s="12">
         <v>0.21</v>
       </c>
-      <c r="I19" s="52"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="31" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H20" s="12">
         <v>0.23</v>
       </c>
-      <c r="I20" s="52"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="31" t="s">
@@ -14393,18 +14401,18 @@
         <v>14</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H21" s="12">
         <v>0.19</v>
       </c>
-      <c r="I21" s="52"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="31" t="s">
@@ -14414,18 +14422,18 @@
         <v>14</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H22" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I22" s="52"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="31" t="s">
@@ -14435,18 +14443,18 @@
         <v>14</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H23" s="12">
         <v>0.5</v>
       </c>
-      <c r="I23" s="52"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="31" t="s">
@@ -14456,13 +14464,13 @@
         <v>14</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H24" s="12">
         <v>0.24</v>
@@ -14470,40 +14478,40 @@
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>36</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H25" s="12">
         <v>0.31</v>
       </c>
-      <c r="I25" s="52"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="31" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="31" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H26" s="12">
         <v>0.25</v>
@@ -14511,19 +14519,19 @@
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="31" t="s">
-        <v>70</v>
+      <c r="G27" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H27" s="12">
         <v>1.1299999999999999</v>
@@ -14531,19 +14539,19 @@
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" s="31" t="s">
         <v>36</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>70</v>
+        <v>77</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H28" s="12">
         <v>0.23</v>
@@ -14551,40 +14559,40 @@
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H29" s="12">
         <v>0.27</v>
       </c>
-      <c r="I29" s="52"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G30" s="31" t="s">
-        <v>70</v>
+      <c r="G30" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H30" s="12">
         <v>0.32</v>
@@ -14592,19 +14600,19 @@
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G31" s="31" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H31" s="12">
         <v>0.18</v>
@@ -14612,19 +14620,19 @@
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F32" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="31" t="s">
-        <v>70</v>
+      <c r="G32" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="H32" s="12">
         <v>0.31</v>
@@ -14638,7 +14646,7 @@
     </row>
   </sheetData>
   <autoFilter ref="C2:G32" xr:uid="{5E3430EC-E785-4A6F-B685-654D51361B6E}"/>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>